<commit_message>
start the coding, therefore changing values in the Assay files
</commit_message>
<xml_diff>
--- a/assays/dilutionSeriesChlamy_ASSAY/isa.assay.xlsx
+++ b/assays/dilutionSeriesChlamy_ASSAY/isa.assay.xlsx
@@ -6,14 +6,13 @@
   <sheets>
     <sheet sheetId="1" name="isa_assay" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="MassSpec" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="NewTable0" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>ASSAY</t>
   </si>
@@ -33,6 +32,9 @@
     <t>Assay Measurement Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Proteomics </t>
+  </si>
+  <si>
     <t>Assay Measurement Type Term Accession Number</t>
   </si>
   <si>
@@ -42,12 +44,21 @@
     <t>Assay Technology Type</t>
   </si>
   <si>
+    <t>mass spectrometry</t>
+  </si>
+  <si>
     <t>Assay Technology Type Term Accession Number</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/C_12421</t>
+  </si>
+  <si>
     <t>Assay Technology Type Term Source REF</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>Assay Technology Platform</t>
   </si>
   <si>
@@ -96,106 +107,70 @@
     <t>Input [Data]</t>
   </si>
   <si>
+    <t>Parameter [Digestion]</t>
+  </si>
+  <si>
+    <t>Term Source REF ()</t>
+  </si>
+  <si>
+    <t>Term Accession Number ()</t>
+  </si>
+  <si>
+    <t>Factor [Ratio Light/Heavy]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term Source REF () </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term Accession Number () </t>
+  </si>
+  <si>
+    <t>Characteristic [Organism]</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C14250)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C14250)</t>
+  </si>
+  <si>
+    <t>Output [Data]</t>
+  </si>
+  <si>
     <t>Data Format</t>
   </si>
   <si>
     <t>Data Selector Format</t>
   </si>
   <si>
-    <t>Parameter [Digestion]</t>
-  </si>
-  <si>
-    <t>Term Source REF ()</t>
-  </si>
-  <si>
-    <t>Term Accession Number ()</t>
-  </si>
-  <si>
-    <t>Factor [Ratio Light/Heavy]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term Source REF () </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term Accession Number () </t>
-  </si>
-  <si>
-    <t>Characteristic [Organism]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NCIT:C14250)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NCIT:C14250)</t>
-  </si>
-  <si>
-    <t>Output [Data]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Format </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Selector Format </t>
-  </si>
-  <si>
-    <t>ChlamyCulture14N</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Trypsin</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Trypsin</t>
-  </si>
-  <si>
-    <t>CHEBI</t>
-  </si>
-  <si>
-    <t>https://bioregistry.io/CHEBI:9765</t>
-  </si>
-  <si>
     <t>0.625</t>
   </si>
   <si>
     <t xml:space="preserve">Chlamy </t>
   </si>
   <si>
-    <t>./assays/dilutionSeries_Chlamy/dataset/20170519 TM FScon3501/20170519 TM FScon3501.wiff</t>
-  </si>
-  <si>
-    <t>ChlamyCulture15N</t>
-  </si>
-  <si>
-    <t>MS</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ols4/ontologies/ms/classes/http%253A%252F%252Fpurl.obolibrary.org%252Fobo%252FMS_1001251</t>
+    <t>./assays/dilutionSeriesChlamy_ASSAY/dataset/20170519 TM FScon3501/20170519 TM FScon3501.wiff</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
   <si>
     <t>0.3125</t>
   </si>
   <si>
-    <t>Input [Sample Name]</t>
-  </si>
-  <si>
-    <t>Parameter [heat]</t>
-  </si>
-  <si>
-    <t>Term Source REF (C:3519)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (C:3519)</t>
-  </si>
-  <si>
-    <t>Output [Sample Name]</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>hot</t>
-  </si>
-  <si>
-    <t>test_1</t>
+    <t>c</t>
+  </si>
+  <si>
+    <t>0.0125</t>
   </si>
 </sst>
 </file>
@@ -251,8 +226,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable0" displayName="annotationTable0" ref="A1:O3" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:O3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable0" displayName="annotationTable0" ref="A1:M4" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:M4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -266,45 +241,21 @@
     <filterColumn colId="10" hiddenButton="1"/>
     <filterColumn colId="11" hiddenButton="1"/>
     <filterColumn colId="12" hiddenButton="1"/>
-    <filterColumn colId="13" hiddenButton="1"/>
-    <filterColumn colId="14" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="15">
+  <tableColumns count="13">
     <tableColumn id="1" name="Input [Data]" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Data Format" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Data Selector Format" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Parameter [Digestion]" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Term Source REF ()" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Term Accession Number ()" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Factor [Ratio Light/Heavy]" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Term Source REF () " totalsRowFunction="none"/>
-    <tableColumn id="9" name="Term Accession Number () " totalsRowFunction="none"/>
-    <tableColumn id="10" name="Characteristic [Organism]" totalsRowFunction="none"/>
-    <tableColumn id="11" name="Term Source REF (NCIT:C14250)" totalsRowFunction="none"/>
-    <tableColumn id="12" name="Term Accession Number (NCIT:C14250)" totalsRowFunction="none"/>
-    <tableColumn id="13" name="Output [Data]" totalsRowFunction="none"/>
-    <tableColumn id="14" name="Data Format " totalsRowFunction="none"/>
-    <tableColumn id="15" name="Data Selector Format " totalsRowFunction="none"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" name="annotationTable1" displayName="annotationTable1" ref="A1:E2" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:E2">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Input [Sample Name]" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Parameter [heat]" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Term Source REF (C:3519)" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Term Accession Number (C:3519)" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Output [Sample Name]" totalsRowFunction="none"/>
+    <tableColumn id="2" name="Parameter [Digestion]" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Term Source REF ()" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Term Accession Number ()" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Factor [Ratio Light/Heavy]" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Term Source REF () " totalsRowFunction="none"/>
+    <tableColumn id="7" name="Term Accession Number () " totalsRowFunction="none"/>
+    <tableColumn id="8" name="Characteristic [Organism]" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Term Source REF (NCIT:C14250)" totalsRowFunction="none"/>
+    <tableColumn id="10" name="Term Accession Number (NCIT:C14250)" totalsRowFunction="none"/>
+    <tableColumn id="11" name="Output [Data]" totalsRowFunction="none"/>
+    <tableColumn id="12" name="Data Format" totalsRowFunction="none"/>
+    <tableColumn id="13" name="Data Selector Format" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -633,107 +584,119 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -744,196 +707,171 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:M4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="L1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>50</v>
       </c>
       <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="G3" t="s">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
         <v>52</v>
       </c>
-      <c r="H3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
         <v>47</v>
       </c>
-      <c r="K3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" t="s">
         <v>48</v>
       </c>
-      <c r="N3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
+      <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding some data and coding
</commit_message>
<xml_diff>
--- a/assays/dilutionSeriesChlamy_ASSAY/isa.assay.xlsx
+++ b/assays/dilutionSeriesChlamy_ASSAY/isa.assay.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>ASSAY</t>
   </si>
@@ -140,6 +140,15 @@
     <t>Term Accession Number (NCIT:C14250)</t>
   </si>
   <si>
+    <t>Parameter [Isotope labeling]</t>
+  </si>
+  <si>
+    <t>Term Source REF (PRIDE:0000310)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (PRIDE:0000310)</t>
+  </si>
+  <si>
     <t>Output [Data]</t>
   </si>
   <si>
@@ -164,6 +173,15 @@
     <t xml:space="preserve">Chlamy </t>
   </si>
   <si>
+    <t>metabolic labelling: heavy N (mainly 15N)</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>https://www.ebi.ac.uk/ols4/ontologies/ms/classes/http%253A%252F%252Fpurl.obolibrary.org%252Fobo%252FMS_1002068</t>
+  </si>
+  <si>
     <t>./assays/dilutionSeriesChlamy_ASSAY/dataset/20170519 TM FScon3501/20170519 TM FScon3501.wiff</t>
   </si>
   <si>
@@ -177,9 +195,6 @@
   </si>
   <si>
     <t>Lys-C</t>
-  </si>
-  <si>
-    <t>MS</t>
   </si>
   <si>
     <t>https://www.ebi.ac.uk/ols4/ontologies/ms/classes/http%253A%252F%252Fpurl.obolibrary.org%252Fobo%252FMS_1001309</t>
@@ -241,8 +256,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable0" displayName="annotationTable0" ref="A1:O4" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:O4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable0" displayName="annotationTable0" ref="A1:R4" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:R4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -258,8 +273,11 @@
     <filterColumn colId="12" hiddenButton="1"/>
     <filterColumn colId="13" hiddenButton="1"/>
     <filterColumn colId="14" hiddenButton="1"/>
+    <filterColumn colId="15" hiddenButton="1"/>
+    <filterColumn colId="16" hiddenButton="1"/>
+    <filterColumn colId="17" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="15">
+  <tableColumns count="18">
     <tableColumn id="1" name="Input [Data]" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Data Format" totalsRowFunction="none"/>
     <tableColumn id="3" name="Data Selector Format" totalsRowFunction="none"/>
@@ -272,9 +290,12 @@
     <tableColumn id="10" name="Characteristic [Organism]" totalsRowFunction="none"/>
     <tableColumn id="11" name="Term Source REF (NCIT:C14250)" totalsRowFunction="none"/>
     <tableColumn id="12" name="Term Accession Number (NCIT:C14250)" totalsRowFunction="none"/>
-    <tableColumn id="13" name="Output [Data]" totalsRowFunction="none"/>
-    <tableColumn id="14" name="Data Format " totalsRowFunction="none"/>
-    <tableColumn id="15" name="Data Selector Format " totalsRowFunction="none"/>
+    <tableColumn id="13" name="Parameter [Isotope labeling]" totalsRowFunction="none"/>
+    <tableColumn id="14" name="Term Source REF (PRIDE:0000310)" totalsRowFunction="none"/>
+    <tableColumn id="15" name="Term Accession Number (PRIDE:0000310)" totalsRowFunction="none"/>
+    <tableColumn id="16" name="Output [Data]" totalsRowFunction="none"/>
+    <tableColumn id="17" name="Data Format " totalsRowFunction="none"/>
+    <tableColumn id="18" name="Data Selector Format " totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -726,10 +747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:R4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -775,146 +796,182 @@
       <c r="O1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="N2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" t="s">
         <v>52</v>
       </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" t="s">
-        <v>49</v>
-      </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="M3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="P3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="N4" t="s">
         <v>54</v>
       </c>
-      <c r="E4" t="s">
+      <c r="O4" t="s">
         <v>55</v>
       </c>
-      <c r="F4" t="s">
+      <c r="P4" t="s">
         <v>56</v>
       </c>
-      <c r="G4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" t="s">
-        <v>46</v>
+      <c r="Q4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>